<commit_message>
ui tweaks. force mitigations positive dmg2
</commit_message>
<xml_diff>
--- a/canflood/_pars/cf_bca_template_01.xlsx
+++ b/canflood/_pars/cf_bca_template_01.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LS\03_TOOLS\CanFlood\_git\canflood\_pars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78943DCB-6F07-4F95-A05B-9781D24CEBF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60880DCD-CD95-459B-A3A5-D61F8B273796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{22523B46-B860-4BF7-85DA-5D08A7A0E489}"/>
   </bookViews>
   <sheets>
     <sheet name="smry" sheetId="2" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
+    <sheet name="legend" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="base_year">smry!$B$14</definedName>
-    <definedName name="ead_total" comment="EAD value from CanFlood">smry!$B$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">data!$A$1:$CZ$23</definedName>
+    <definedName name="base_year">smry!$B$15</definedName>
+    <definedName name="ead_baseline" comment="ead of baseline (risk w/o option)">smry!$B$11</definedName>
+    <definedName name="ead_option" comment="EAD value for scenario from CanFlood">smry!$B$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">data!$A$1:$CZ$24</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">data!$A:$B</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,8 +38,173 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>cefect</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{70FC62A3-9E6F-4455-8719-BF23DF6A1E86}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>cefect:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+cells in this column provide a total of the values to the right</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{17F16C39-DF82-4399-8E0A-D629924B4957}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>cefect:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+populate these cells with the development costs for this option</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{86E7D652-BB62-4F77-9B06-BC9A1EE49157}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>cefect:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+populate these cells with the operating costs for the option</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{E3C5C250-1D4C-4030-B4B6-3A7D89A00C6F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>cefect:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ensure 'baseline' values are negative</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{45BF531C-91B5-4A9B-BDDF-62DA238C356B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>cefect:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+populate these cells with the baseline and option EAD values, and any additional benefits. 
+Use Excel's 'named' variables feature to reference values on the 'smry' tab</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>cefect</author>
+  </authors>
+  <commentList>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{BEAFBF73-2E8B-4FAD-A461-B7AFFF8D1A94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>cefect:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This cell has a note</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Total</t>
   </si>
@@ -67,9 +234,6 @@
   </si>
   <si>
     <t>Flood Loss Avoidance</t>
-  </si>
-  <si>
-    <t>risk model EAD</t>
   </si>
   <si>
     <t>other monetized benefits</t>
@@ -111,12 +275,6 @@
     <t>control_filename</t>
   </si>
   <si>
-    <t>ead_total</t>
-  </si>
-  <si>
-    <t>test name</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
@@ -131,16 +289,41 @@
   <si>
     <t>NPV $</t>
   </si>
+  <si>
+    <t>ead_baseline</t>
+  </si>
+  <si>
+    <t>ead_option</t>
+  </si>
+  <si>
+    <t>option EAD</t>
+  </si>
+  <si>
+    <t>baseline EAD</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>cell with a note</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -209,6 +392,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -297,7 +497,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -306,8 +506,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -408,8 +609,13 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="11" fontId="5" fillId="2" borderId="3" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="5"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
+    <cellStyle name="Currency" xfId="8" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="6" builtinId="53"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
@@ -430,6 +636,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -729,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7540B8A-D226-4DE7-8D1D-ECC682EFB196}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A18" sqref="A18:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -743,113 +953,119 @@
   <sheetData>
     <row r="1" spans="1:2" s="31" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="31" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="36"/>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="31" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
+      <c r="B15">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
-        <v>26</v>
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="33">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="31" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="33">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B16" s="32"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="35">
-        <f>NPV(B15, data!E22:CZ22)+data!D22</f>
-        <v>0</v>
-      </c>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="32"/>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="35">
-        <f>NPV(B15, data!E16:CZ16)+data!D16</f>
-        <v>391464275.19412291</v>
+        <f>NPV(B16, data!E23:CZ23)+data!D23</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B19" s="35">
-        <f>B17-B18</f>
-        <v>-391464275.19412291</v>
+        <f>NPV(B16, data!E16:CZ16)+data!D16</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="35">
+        <f>B18-B19</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="34">
-        <f>B17/B18</f>
-        <v>0</v>
+      <c r="B22" s="34" t="e">
+        <f>B18/B19</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -858,11 +1074,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CZ36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CZ37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -878,7 +1094,7 @@
     <row r="1" spans="1:104" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="7">
         <f>base_year</f>
@@ -1810,314 +2026,112 @@
       </c>
       <c r="B4" s="22">
         <f>SUM(D4:CZ4)</f>
-        <v>463401085</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="23">
-        <v>2896367</v>
-      </c>
-      <c r="E4" s="23">
-        <v>3804511</v>
-      </c>
-      <c r="F4" s="23">
-        <v>15930667</v>
-      </c>
-      <c r="G4" s="23">
-        <v>9318157</v>
-      </c>
-      <c r="H4" s="23">
-        <v>7836285</v>
-      </c>
-      <c r="I4" s="23">
-        <v>77604296</v>
-      </c>
-      <c r="J4" s="23">
-        <v>70757375</v>
-      </c>
-      <c r="K4" s="23">
-        <v>111508984</v>
-      </c>
-      <c r="L4" s="23">
-        <v>72109156</v>
-      </c>
-      <c r="M4" s="23">
-        <v>91635287</v>
-      </c>
-      <c r="N4" s="23">
-        <v>0</v>
-      </c>
-      <c r="O4" s="23">
-        <v>0</v>
-      </c>
-      <c r="P4" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="23">
-        <v>0</v>
-      </c>
-      <c r="R4" s="23">
-        <v>0</v>
-      </c>
-      <c r="S4" s="23">
-        <v>0</v>
-      </c>
-      <c r="T4" s="23">
-        <v>0</v>
-      </c>
-      <c r="U4" s="23">
-        <v>0</v>
-      </c>
-      <c r="V4" s="23">
-        <v>0</v>
-      </c>
-      <c r="W4" s="23">
-        <v>0</v>
-      </c>
-      <c r="X4" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AY4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AZ4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BA4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BB4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BC4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BD4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BF4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BG4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BH4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BI4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BK4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BM4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BN4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BO4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BP4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BQ4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BR4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BS4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BT4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BU4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BV4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BW4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BX4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BY4" s="23">
-        <v>0</v>
-      </c>
-      <c r="BZ4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CA4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CB4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CC4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CD4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CE4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CF4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CG4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CH4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CI4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CJ4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CK4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CL4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CM4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CN4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CO4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CP4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CQ4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CR4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CS4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CT4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CU4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CV4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CW4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CX4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CY4" s="23">
-        <v>0</v>
-      </c>
-      <c r="CZ4" s="23">
-        <v>0</v>
-      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="23"/>
+      <c r="AN4" s="23"/>
+      <c r="AO4" s="23"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="23"/>
+      <c r="AR4" s="23"/>
+      <c r="AS4" s="23"/>
+      <c r="AT4" s="23"/>
+      <c r="AU4" s="23"/>
+      <c r="AV4" s="23"/>
+      <c r="AW4" s="23"/>
+      <c r="AX4" s="23"/>
+      <c r="AY4" s="23"/>
+      <c r="AZ4" s="23"/>
+      <c r="BA4" s="23"/>
+      <c r="BB4" s="23"/>
+      <c r="BC4" s="23"/>
+      <c r="BD4" s="23"/>
+      <c r="BE4" s="23"/>
+      <c r="BF4" s="23"/>
+      <c r="BG4" s="23"/>
+      <c r="BH4" s="23"/>
+      <c r="BI4" s="23"/>
+      <c r="BJ4" s="23"/>
+      <c r="BK4" s="23"/>
+      <c r="BL4" s="23"/>
+      <c r="BM4" s="23"/>
+      <c r="BN4" s="23"/>
+      <c r="BO4" s="23"/>
+      <c r="BP4" s="23"/>
+      <c r="BQ4" s="23"/>
+      <c r="BR4" s="23"/>
+      <c r="BS4" s="23"/>
+      <c r="BT4" s="23"/>
+      <c r="BU4" s="23"/>
+      <c r="BV4" s="23"/>
+      <c r="BW4" s="23"/>
+      <c r="BX4" s="23"/>
+      <c r="BY4" s="23"/>
+      <c r="BZ4" s="23"/>
+      <c r="CA4" s="23"/>
+      <c r="CB4" s="23"/>
+      <c r="CC4" s="23"/>
+      <c r="CD4" s="23"/>
+      <c r="CE4" s="23"/>
+      <c r="CF4" s="23"/>
+      <c r="CG4" s="23"/>
+      <c r="CH4" s="23"/>
+      <c r="CI4" s="23"/>
+      <c r="CJ4" s="23"/>
+      <c r="CK4" s="23"/>
+      <c r="CL4" s="23"/>
+      <c r="CM4" s="23"/>
+      <c r="CN4" s="23"/>
+      <c r="CO4" s="23"/>
+      <c r="CP4" s="23"/>
+      <c r="CQ4" s="23"/>
+      <c r="CR4" s="23"/>
+      <c r="CS4" s="23"/>
+      <c r="CT4" s="23"/>
+      <c r="CU4" s="23"/>
+      <c r="CV4" s="23"/>
+      <c r="CW4" s="23"/>
+      <c r="CX4" s="23"/>
+      <c r="CY4" s="23"/>
+      <c r="CZ4" s="23"/>
     </row>
     <row r="5" spans="1:104" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -2459,50 +2473,50 @@
       </c>
       <c r="B8" s="26">
         <f>SUM(D8:CZ8)</f>
-        <v>463401085</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="20">
         <f>SUM(D4:D7)</f>
-        <v>2896367</v>
+        <v>0</v>
       </c>
       <c r="E8" s="20">
         <f t="shared" ref="E8:J8" si="6">SUM(E4:E7)</f>
-        <v>3804511</v>
+        <v>0</v>
       </c>
       <c r="F8" s="20">
         <f t="shared" si="6"/>
-        <v>15930667</v>
+        <v>0</v>
       </c>
       <c r="G8" s="20">
         <f t="shared" si="6"/>
-        <v>9318157</v>
+        <v>0</v>
       </c>
       <c r="H8" s="20">
         <f t="shared" si="6"/>
-        <v>7836285</v>
+        <v>0</v>
       </c>
       <c r="I8" s="20">
         <f t="shared" si="6"/>
-        <v>77604296</v>
+        <v>0</v>
       </c>
       <c r="J8" s="20">
         <f t="shared" si="6"/>
-        <v>70757375</v>
+        <v>0</v>
       </c>
       <c r="K8" s="20">
         <f t="shared" ref="K8" si="7">SUM(K4:K7)</f>
-        <v>111508984</v>
+        <v>0</v>
       </c>
       <c r="L8" s="20">
         <f t="shared" ref="L8" si="8">SUM(L4:L7)</f>
-        <v>72109156</v>
+        <v>0</v>
       </c>
       <c r="M8" s="20">
         <f t="shared" ref="M8" si="9">SUM(M4:M7)</f>
-        <v>91635287</v>
+        <v>0</v>
       </c>
       <c r="N8" s="20">
         <f t="shared" ref="N8" si="10">SUM(N4:N7)</f>
@@ -2891,314 +2905,112 @@
       </c>
       <c r="B11" s="22">
         <f>SUM(D11:CZ11)</f>
-        <v>196725000</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="23">
-        <v>0</v>
-      </c>
-      <c r="E11" s="23">
-        <v>0</v>
-      </c>
-      <c r="F11" s="23">
-        <v>0</v>
-      </c>
-      <c r="G11" s="23">
-        <v>0</v>
-      </c>
-      <c r="H11" s="23">
-        <v>0</v>
-      </c>
-      <c r="I11" s="23">
-        <v>0</v>
-      </c>
-      <c r="J11" s="23">
-        <v>0</v>
-      </c>
-      <c r="K11" s="23">
-        <v>0</v>
-      </c>
-      <c r="L11" s="23">
-        <v>0</v>
-      </c>
-      <c r="M11" s="23">
-        <v>0</v>
-      </c>
-      <c r="N11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="O11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="P11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="Q11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="R11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="S11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="T11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="U11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="V11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="W11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="X11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="Y11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="Z11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AA11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AB11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AC11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AD11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AE11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AF11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AG11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="AH11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AI11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AJ11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AK11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AL11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AM11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AN11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AO11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AP11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AQ11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="AR11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AS11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AT11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AU11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AV11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AW11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AX11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AY11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="AZ11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BA11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="BB11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BC11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BD11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BE11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BF11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BG11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BH11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BI11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BJ11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BK11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="BL11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BM11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BN11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BO11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BP11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BQ11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BR11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BS11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BT11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BU11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="BV11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BW11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BX11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BY11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="BZ11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CA11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CB11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CC11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CD11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CE11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="CF11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CG11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CH11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CI11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CJ11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CK11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CL11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CM11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CN11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CO11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="CP11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CQ11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CR11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CS11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CT11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CU11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CV11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CW11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CX11" s="23">
-        <v>975000</v>
-      </c>
-      <c r="CY11" s="23">
-        <v>12975000</v>
-      </c>
-      <c r="CZ11" s="23">
-        <v>975000</v>
-      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="23"/>
+      <c r="AE11" s="23"/>
+      <c r="AF11" s="23"/>
+      <c r="AG11" s="23"/>
+      <c r="AH11" s="23"/>
+      <c r="AI11" s="23"/>
+      <c r="AJ11" s="23"/>
+      <c r="AK11" s="23"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
+      <c r="AN11" s="23"/>
+      <c r="AO11" s="23"/>
+      <c r="AP11" s="23"/>
+      <c r="AQ11" s="23"/>
+      <c r="AR11" s="23"/>
+      <c r="AS11" s="23"/>
+      <c r="AT11" s="23"/>
+      <c r="AU11" s="23"/>
+      <c r="AV11" s="23"/>
+      <c r="AW11" s="23"/>
+      <c r="AX11" s="23"/>
+      <c r="AY11" s="23"/>
+      <c r="AZ11" s="23"/>
+      <c r="BA11" s="23"/>
+      <c r="BB11" s="23"/>
+      <c r="BC11" s="23"/>
+      <c r="BD11" s="23"/>
+      <c r="BE11" s="23"/>
+      <c r="BF11" s="23"/>
+      <c r="BG11" s="23"/>
+      <c r="BH11" s="23"/>
+      <c r="BI11" s="23"/>
+      <c r="BJ11" s="23"/>
+      <c r="BK11" s="23"/>
+      <c r="BL11" s="23"/>
+      <c r="BM11" s="23"/>
+      <c r="BN11" s="23"/>
+      <c r="BO11" s="23"/>
+      <c r="BP11" s="23"/>
+      <c r="BQ11" s="23"/>
+      <c r="BR11" s="23"/>
+      <c r="BS11" s="23"/>
+      <c r="BT11" s="23"/>
+      <c r="BU11" s="23"/>
+      <c r="BV11" s="23"/>
+      <c r="BW11" s="23"/>
+      <c r="BX11" s="23"/>
+      <c r="BY11" s="23"/>
+      <c r="BZ11" s="23"/>
+      <c r="CA11" s="23"/>
+      <c r="CB11" s="23"/>
+      <c r="CC11" s="23"/>
+      <c r="CD11" s="23"/>
+      <c r="CE11" s="23"/>
+      <c r="CF11" s="23"/>
+      <c r="CG11" s="23"/>
+      <c r="CH11" s="23"/>
+      <c r="CI11" s="23"/>
+      <c r="CJ11" s="23"/>
+      <c r="CK11" s="23"/>
+      <c r="CL11" s="23"/>
+      <c r="CM11" s="23"/>
+      <c r="CN11" s="23"/>
+      <c r="CO11" s="23"/>
+      <c r="CP11" s="23"/>
+      <c r="CQ11" s="23"/>
+      <c r="CR11" s="23"/>
+      <c r="CS11" s="23"/>
+      <c r="CT11" s="23"/>
+      <c r="CU11" s="23"/>
+      <c r="CV11" s="23"/>
+      <c r="CW11" s="23"/>
+      <c r="CX11" s="23"/>
+      <c r="CY11" s="23"/>
+      <c r="CZ11" s="23"/>
     </row>
     <row r="12" spans="1:104" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
@@ -3427,7 +3239,7 @@
       </c>
       <c r="B14" s="26">
         <f>SUM(D14:CZ14)</f>
-        <v>196725000</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>0</v>
@@ -3474,367 +3286,367 @@
       </c>
       <c r="N14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="O14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="P14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="R14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="S14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="T14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="U14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="V14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="W14" s="20">
         <f t="shared" si="86"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="X14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="20">
         <f t="shared" si="86"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="AH14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AI14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AJ14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AK14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AN14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AO14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AP14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AQ14" s="20">
         <f t="shared" si="86"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="AR14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AS14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AT14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AU14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AV14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AW14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AX14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AY14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AZ14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BA14" s="20">
         <f t="shared" si="86"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="BB14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BD14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BE14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BG14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BH14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BI14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BJ14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BK14" s="20">
         <f t="shared" si="86"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="BL14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BM14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BN14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BO14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BP14" s="20">
         <f t="shared" si="86"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BQ14" s="20">
         <f t="shared" ref="BQ14:CZ14" si="87">SUM(BQ11:BQ12)</f>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BR14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BS14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BT14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BU14" s="20">
         <f t="shared" si="87"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="BV14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BW14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BX14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BY14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BZ14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CA14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CB14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CC14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CD14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CE14" s="20">
         <f t="shared" si="87"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="CF14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CG14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CH14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CI14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CJ14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CK14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CL14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CM14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CN14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CO14" s="20">
         <f t="shared" si="87"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="CP14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CQ14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CR14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CS14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CT14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CU14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CV14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CW14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CX14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CY14" s="20">
         <f t="shared" si="87"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="CZ14" s="20">
         <f t="shared" si="87"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:104" s="16" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -3947,418 +3759,418 @@
     </row>
     <row r="16" spans="1:104" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="26">
         <f>SUM(D16:CZ16)</f>
-        <v>660126085</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="20">
         <f t="shared" ref="D16:AI16" si="88">D14+D8</f>
-        <v>2896367</v>
+        <v>0</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="88"/>
-        <v>3804511</v>
+        <v>0</v>
       </c>
       <c r="F16" s="20">
         <f t="shared" si="88"/>
-        <v>15930667</v>
+        <v>0</v>
       </c>
       <c r="G16" s="20">
         <f t="shared" si="88"/>
-        <v>9318157</v>
+        <v>0</v>
       </c>
       <c r="H16" s="20">
         <f t="shared" si="88"/>
-        <v>7836285</v>
+        <v>0</v>
       </c>
       <c r="I16" s="20">
         <f t="shared" si="88"/>
-        <v>77604296</v>
+        <v>0</v>
       </c>
       <c r="J16" s="20">
         <f t="shared" si="88"/>
-        <v>70757375</v>
+        <v>0</v>
       </c>
       <c r="K16" s="20">
         <f t="shared" si="88"/>
-        <v>111508984</v>
+        <v>0</v>
       </c>
       <c r="L16" s="20">
         <f t="shared" si="88"/>
-        <v>72109156</v>
+        <v>0</v>
       </c>
       <c r="M16" s="20">
         <f t="shared" si="88"/>
-        <v>91635287</v>
+        <v>0</v>
       </c>
       <c r="N16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="O16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="P16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="R16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="S16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="T16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="U16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="V16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="W16" s="20">
         <f t="shared" si="88"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="X16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AB16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AC16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AD16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AE16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AF16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AG16" s="20">
         <f t="shared" si="88"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="AH16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AI16" s="20">
         <f t="shared" si="88"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AJ16" s="20">
         <f t="shared" ref="AJ16:BO16" si="89">AJ14+AJ8</f>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AK16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AM16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AN16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AO16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AP16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AQ16" s="20">
         <f t="shared" si="89"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="AR16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AS16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AT16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AU16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AV16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AW16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AX16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AY16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="AZ16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BA16" s="20">
         <f t="shared" si="89"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="BB16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BC16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BD16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BE16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BF16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BG16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BH16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BI16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BJ16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BK16" s="20">
         <f t="shared" si="89"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="BL16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BM16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BN16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BO16" s="20">
         <f t="shared" si="89"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BP16" s="20">
         <f t="shared" ref="BP16:CZ16" si="90">BP14+BP8</f>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BQ16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BR16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BS16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BT16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BU16" s="20">
         <f t="shared" si="90"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="BV16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BW16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BX16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BY16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="BZ16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CA16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CB16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CC16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CD16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CE16" s="20">
         <f t="shared" si="90"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="CF16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CG16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CH16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CI16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CJ16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CK16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CL16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CM16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CN16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CO16" s="20">
         <f t="shared" si="90"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="CP16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CQ16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CR16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CS16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CT16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CU16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CV16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CW16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CX16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
       <c r="CY16" s="20">
         <f t="shared" si="90"/>
-        <v>12975000</v>
+        <v>0</v>
       </c>
       <c r="CZ16" s="20">
         <f t="shared" si="90"/>
-        <v>975000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:104" s="16" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -4581,414 +4393,421 @@
     </row>
     <row r="19" spans="1:104" s="16" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B19" s="22">
         <f>SUM(D19:CZ19)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="E19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="F19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="G19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="H19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="I19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="J19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="K19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="L19" s="23">
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="M19" s="23">
-        <f>ead_total*0.5</f>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="N19" s="23">
-        <f t="shared" ref="N19:AS19" si="91">ead_total</f>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="O19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="P19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="Q19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="R19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="S19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="T19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="U19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="V19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="W19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="X19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="Y19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="Z19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AA19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AB19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AC19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AD19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AE19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AF19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AG19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AH19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AI19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AJ19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AK19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AL19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AM19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AN19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AO19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AP19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AQ19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AR19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AS19" s="23">
-        <f t="shared" si="91"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AT19" s="23">
-        <f t="shared" ref="AT19:BY19" si="92">ead_total</f>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AU19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AV19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AW19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AX19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AY19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="AZ19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BA19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BB19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BC19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BD19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BE19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BF19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BG19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BH19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BI19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BJ19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BK19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BL19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BM19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BN19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BO19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BP19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BQ19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BR19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BS19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BT19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BU19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BV19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BW19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BX19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BY19" s="23">
-        <f t="shared" si="92"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="BZ19" s="23">
-        <f t="shared" ref="BZ19:CZ19" si="93">ead_total</f>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CA19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CB19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CC19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CD19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CE19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CF19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CG19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CH19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CI19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CJ19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CK19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CL19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CM19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CN19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CO19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CP19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CQ19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CR19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CS19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CT19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CU19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CV19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CW19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CX19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CY19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
       <c r="CZ19" s="23">
-        <f t="shared" si="93"/>
+        <f>-ead_baseline</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:104" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B20" s="22">
         <f>SUM(D20:CZ20)</f>
@@ -4998,945 +4817,1156 @@
         <v>0</v>
       </c>
       <c r="D20" s="23">
+        <f t="shared" ref="D20:M20" si="91">ead_option</f>
         <v>0</v>
       </c>
       <c r="E20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="F20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="G20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="H20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="I20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="J20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="K20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="M20" s="23">
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="N20" s="23">
+        <f t="shared" ref="N20:AS20" si="92">ead_option</f>
         <v>0</v>
       </c>
       <c r="O20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="P20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="Q20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="R20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="S20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="T20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="U20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="V20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="W20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="X20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="Y20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="Z20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AA20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AB20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AC20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AD20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AE20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AF20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AG20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AH20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AI20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AJ20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AK20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AL20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AM20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AN20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AO20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AP20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AQ20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AR20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AS20" s="23">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AT20" s="23">
+        <f t="shared" ref="AT20:BY20" si="93">ead_option</f>
         <v>0</v>
       </c>
       <c r="AU20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AV20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AW20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AX20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AY20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AZ20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BA20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BB20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BC20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BD20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BE20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BF20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BG20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BH20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BI20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BJ20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BK20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BL20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BM20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BN20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BO20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BP20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BQ20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BR20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BS20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BT20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BU20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BV20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BW20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BX20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BY20" s="23">
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="BZ20" s="23">
+        <f t="shared" ref="BZ20:CZ20" si="94">ead_option</f>
         <v>0</v>
       </c>
       <c r="CA20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CB20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CC20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CD20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CE20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CF20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CG20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CH20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CI20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CJ20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CK20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CL20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CM20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CN20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CO20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CP20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CQ20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CR20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CS20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CT20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CU20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CV20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CW20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CX20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CY20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="CZ20" s="23">
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:104" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
+    <row r="21" spans="1:104" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="22">
+        <f>SUM(D21:CZ21)</f>
+        <v>0</v>
+      </c>
       <c r="C21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
-      <c r="AA21" s="15"/>
-      <c r="AB21" s="15"/>
-      <c r="AC21" s="15"/>
-      <c r="AD21" s="15"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="15"/>
-      <c r="AG21" s="15"/>
-      <c r="AH21" s="15"/>
-      <c r="AI21" s="15"/>
-      <c r="AJ21" s="15"/>
-      <c r="AK21" s="15"/>
-      <c r="AL21" s="15"/>
-      <c r="AM21" s="15"/>
-      <c r="AN21" s="15"/>
-      <c r="AO21" s="15"/>
-      <c r="AP21" s="15"/>
-      <c r="AQ21" s="15"/>
-      <c r="AR21" s="15"/>
-      <c r="AS21" s="15"/>
-      <c r="AT21" s="15"/>
-      <c r="AU21" s="15"/>
-      <c r="AV21" s="15"/>
-      <c r="AW21" s="15"/>
-      <c r="AX21" s="15"/>
-      <c r="AY21" s="15"/>
-      <c r="AZ21" s="15"/>
-      <c r="BA21" s="15"/>
-      <c r="BB21" s="15"/>
-      <c r="BC21" s="15"/>
-      <c r="BD21" s="15"/>
-      <c r="BE21" s="15"/>
-      <c r="BF21" s="15"/>
-      <c r="BG21" s="15"/>
-      <c r="BH21" s="15"/>
-      <c r="BI21" s="15"/>
-      <c r="BJ21" s="15"/>
-      <c r="BK21" s="15"/>
-      <c r="BL21" s="15"/>
-      <c r="BM21" s="15"/>
-      <c r="BN21" s="15"/>
-      <c r="BO21" s="15"/>
-      <c r="BP21" s="15"/>
-      <c r="BQ21" s="15"/>
-      <c r="BR21" s="15"/>
-      <c r="BS21" s="15"/>
-      <c r="BT21" s="15"/>
-      <c r="BU21" s="15"/>
-      <c r="BV21" s="15"/>
-      <c r="BW21" s="15"/>
-      <c r="BX21" s="15"/>
-      <c r="BY21" s="15"/>
-      <c r="BZ21" s="15"/>
-      <c r="CA21" s="15"/>
-      <c r="CB21" s="15"/>
-      <c r="CC21" s="15"/>
-      <c r="CD21" s="15"/>
-      <c r="CE21" s="15"/>
-      <c r="CF21" s="15"/>
-      <c r="CG21" s="15"/>
-      <c r="CH21" s="15"/>
-      <c r="CI21" s="15"/>
-      <c r="CJ21" s="15"/>
-      <c r="CK21" s="15"/>
-      <c r="CL21" s="15"/>
-      <c r="CM21" s="15"/>
-      <c r="CN21" s="15"/>
-      <c r="CO21" s="15"/>
-      <c r="CP21" s="15"/>
-      <c r="CQ21" s="15"/>
-      <c r="CR21" s="15"/>
-      <c r="CS21" s="15"/>
-      <c r="CT21" s="15"/>
-      <c r="CU21" s="15"/>
-      <c r="CV21" s="15"/>
-      <c r="CW21" s="15"/>
-      <c r="CX21" s="15"/>
-      <c r="CY21" s="15"/>
-      <c r="CZ21" s="15"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+      <c r="AD21" s="23"/>
+      <c r="AE21" s="23"/>
+      <c r="AF21" s="23"/>
+      <c r="AG21" s="23"/>
+      <c r="AH21" s="23"/>
+      <c r="AI21" s="23"/>
+      <c r="AJ21" s="23"/>
+      <c r="AK21" s="23"/>
+      <c r="AL21" s="23"/>
+      <c r="AM21" s="23"/>
+      <c r="AN21" s="23"/>
+      <c r="AO21" s="23"/>
+      <c r="AP21" s="23"/>
+      <c r="AQ21" s="23"/>
+      <c r="AR21" s="23"/>
+      <c r="AS21" s="23"/>
+      <c r="AT21" s="23"/>
+      <c r="AU21" s="23"/>
+      <c r="AV21" s="23"/>
+      <c r="AW21" s="23"/>
+      <c r="AX21" s="23"/>
+      <c r="AY21" s="23"/>
+      <c r="AZ21" s="23"/>
+      <c r="BA21" s="23"/>
+      <c r="BB21" s="23"/>
+      <c r="BC21" s="23"/>
+      <c r="BD21" s="23"/>
+      <c r="BE21" s="23"/>
+      <c r="BF21" s="23"/>
+      <c r="BG21" s="23"/>
+      <c r="BH21" s="23"/>
+      <c r="BI21" s="23"/>
+      <c r="BJ21" s="23"/>
+      <c r="BK21" s="23"/>
+      <c r="BL21" s="23"/>
+      <c r="BM21" s="23"/>
+      <c r="BN21" s="23"/>
+      <c r="BO21" s="23"/>
+      <c r="BP21" s="23"/>
+      <c r="BQ21" s="23"/>
+      <c r="BR21" s="23"/>
+      <c r="BS21" s="23"/>
+      <c r="BT21" s="23"/>
+      <c r="BU21" s="23"/>
+      <c r="BV21" s="23"/>
+      <c r="BW21" s="23"/>
+      <c r="BX21" s="23"/>
+      <c r="BY21" s="23"/>
+      <c r="BZ21" s="23"/>
+      <c r="CA21" s="23"/>
+      <c r="CB21" s="23"/>
+      <c r="CC21" s="23"/>
+      <c r="CD21" s="23"/>
+      <c r="CE21" s="23"/>
+      <c r="CF21" s="23"/>
+      <c r="CG21" s="23"/>
+      <c r="CH21" s="23"/>
+      <c r="CI21" s="23"/>
+      <c r="CJ21" s="23"/>
+      <c r="CK21" s="23"/>
+      <c r="CL21" s="23"/>
+      <c r="CM21" s="23"/>
+      <c r="CN21" s="23"/>
+      <c r="CO21" s="23"/>
+      <c r="CP21" s="23"/>
+      <c r="CQ21" s="23"/>
+      <c r="CR21" s="23"/>
+      <c r="CS21" s="23"/>
+      <c r="CT21" s="23"/>
+      <c r="CU21" s="23"/>
+      <c r="CV21" s="23"/>
+      <c r="CW21" s="23"/>
+      <c r="CX21" s="23"/>
+      <c r="CY21" s="23"/>
+      <c r="CZ21" s="23"/>
     </row>
-    <row r="22" spans="1:104" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="26">
-        <f>SUM(D22:CZ22)</f>
-        <v>0</v>
-      </c>
+    <row r="22" spans="1:104" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="15"/>
+      <c r="AH22" s="15"/>
+      <c r="AI22" s="15"/>
+      <c r="AJ22" s="15"/>
+      <c r="AK22" s="15"/>
+      <c r="AL22" s="15"/>
+      <c r="AM22" s="15"/>
+      <c r="AN22" s="15"/>
+      <c r="AO22" s="15"/>
+      <c r="AP22" s="15"/>
+      <c r="AQ22" s="15"/>
+      <c r="AR22" s="15"/>
+      <c r="AS22" s="15"/>
+      <c r="AT22" s="15"/>
+      <c r="AU22" s="15"/>
+      <c r="AV22" s="15"/>
+      <c r="AW22" s="15"/>
+      <c r="AX22" s="15"/>
+      <c r="AY22" s="15"/>
+      <c r="AZ22" s="15"/>
+      <c r="BA22" s="15"/>
+      <c r="BB22" s="15"/>
+      <c r="BC22" s="15"/>
+      <c r="BD22" s="15"/>
+      <c r="BE22" s="15"/>
+      <c r="BF22" s="15"/>
+      <c r="BG22" s="15"/>
+      <c r="BH22" s="15"/>
+      <c r="BI22" s="15"/>
+      <c r="BJ22" s="15"/>
+      <c r="BK22" s="15"/>
+      <c r="BL22" s="15"/>
+      <c r="BM22" s="15"/>
+      <c r="BN22" s="15"/>
+      <c r="BO22" s="15"/>
+      <c r="BP22" s="15"/>
+      <c r="BQ22" s="15"/>
+      <c r="BR22" s="15"/>
+      <c r="BS22" s="15"/>
+      <c r="BT22" s="15"/>
+      <c r="BU22" s="15"/>
+      <c r="BV22" s="15"/>
+      <c r="BW22" s="15"/>
+      <c r="BX22" s="15"/>
+      <c r="BY22" s="15"/>
+      <c r="BZ22" s="15"/>
+      <c r="CA22" s="15"/>
+      <c r="CB22" s="15"/>
+      <c r="CC22" s="15"/>
+      <c r="CD22" s="15"/>
+      <c r="CE22" s="15"/>
+      <c r="CF22" s="15"/>
+      <c r="CG22" s="15"/>
+      <c r="CH22" s="15"/>
+      <c r="CI22" s="15"/>
+      <c r="CJ22" s="15"/>
+      <c r="CK22" s="15"/>
+      <c r="CL22" s="15"/>
+      <c r="CM22" s="15"/>
+      <c r="CN22" s="15"/>
+      <c r="CO22" s="15"/>
+      <c r="CP22" s="15"/>
+      <c r="CQ22" s="15"/>
+      <c r="CR22" s="15"/>
+      <c r="CS22" s="15"/>
+      <c r="CT22" s="15"/>
+      <c r="CU22" s="15"/>
+      <c r="CV22" s="15"/>
+      <c r="CW22" s="15"/>
+      <c r="CX22" s="15"/>
+      <c r="CY22" s="15"/>
+      <c r="CZ22" s="15"/>
+    </row>
+    <row r="23" spans="1:104" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="26">
+        <f>SUM(D23:CZ23)</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D22" s="20">
-        <f>SUM(D19:D20)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="20">
-        <f t="shared" ref="E22:BP22" si="94">SUM(E19:E20)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="S22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="T22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="U22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="V22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="W22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="X22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="Y22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="Z22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AA22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AB22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AC22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AD22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AE22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AF22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AG22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AH22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AI22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AK22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AL22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AM22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AN22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AO22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AP22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AQ22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AR22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AS22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AT22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AU22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AV22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AW22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AX22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AY22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="AZ22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BA22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BB22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BC22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BD22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BE22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BF22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BG22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BH22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BI22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BJ22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BK22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BL22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BM22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BN22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BO22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BP22" s="20">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="BQ22" s="20">
-        <f t="shared" ref="BQ22:CZ22" si="95">SUM(BQ19:BQ20)</f>
-        <v>0</v>
-      </c>
-      <c r="BR22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="BS22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="BT22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="BU22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="BV22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="BW22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="BX22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="BY22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="BZ22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CA22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CB22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CC22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CD22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CE22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CF22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CG22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CH22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CI22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CJ22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CK22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CL22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CM22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CN22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CO22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CP22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CQ22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CR22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CS22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CT22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CU22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CV22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CW22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CX22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CY22" s="20">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="CZ22" s="20">
-        <f t="shared" si="95"/>
+      <c r="D23" s="20">
+        <f>SUM(D19:D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="20">
+        <f t="shared" ref="E23:BP23" si="95">SUM(E19:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="W23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="X23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AE23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AG23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AH23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AI23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AK23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AL23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AM23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AN23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AO23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AP23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AR23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AS23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AT23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AU23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AV23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AW23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AX23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AY23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="AZ23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BA23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BB23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BC23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BD23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BE23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BF23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BG23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BH23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BI23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BJ23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BK23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BL23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BM23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BN23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BO23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BP23" s="20">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="BQ23" s="20">
+        <f t="shared" ref="BQ23:CZ23" si="96">SUM(BQ19:BQ21)</f>
+        <v>0</v>
+      </c>
+      <c r="BR23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="BS23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="BT23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="BU23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="BV23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="BW23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="BX23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="BY23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="BZ23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CA23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CB23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CC23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CD23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CE23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CF23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CG23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CH23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CI23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CJ23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CK23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CL23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CM23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CN23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CO23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CP23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CQ23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CR23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CS23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CT23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CU23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CV23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CW23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CX23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CY23" s="20">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="CZ23" s="20">
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:104" s="16" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-      <c r="AA23" s="15"/>
-      <c r="AB23" s="15"/>
-      <c r="AC23" s="15"/>
-      <c r="AD23" s="15"/>
-      <c r="AE23" s="15"/>
-      <c r="AF23" s="15"/>
-      <c r="AG23" s="15"/>
-      <c r="AH23" s="15"/>
-      <c r="AI23" s="15"/>
-      <c r="AJ23" s="15"/>
-      <c r="AK23" s="15"/>
-      <c r="AL23" s="15"/>
-      <c r="AM23" s="15"/>
-      <c r="AN23" s="15"/>
-      <c r="AO23" s="15"/>
-      <c r="AP23" s="15"/>
-      <c r="AQ23" s="15"/>
-      <c r="AR23" s="15"/>
-      <c r="AS23" s="15"/>
-      <c r="AT23" s="15"/>
-      <c r="AU23" s="15"/>
-      <c r="AV23" s="15"/>
-      <c r="AW23" s="15"/>
-      <c r="AX23" s="15"/>
-      <c r="AY23" s="15"/>
-      <c r="AZ23" s="15"/>
-      <c r="BA23" s="15"/>
-      <c r="BB23" s="15"/>
-      <c r="BC23" s="15"/>
-      <c r="BD23" s="15"/>
-      <c r="BE23" s="15"/>
-      <c r="BF23" s="15"/>
-      <c r="BG23" s="15"/>
-      <c r="BH23" s="15"/>
-      <c r="BI23" s="15"/>
-      <c r="BJ23" s="15"/>
-      <c r="BK23" s="15"/>
-      <c r="BL23" s="15"/>
-      <c r="BM23" s="15"/>
-      <c r="BN23" s="15"/>
-      <c r="BO23" s="15"/>
-      <c r="BP23" s="15"/>
-      <c r="BQ23" s="15"/>
-      <c r="BR23" s="15"/>
-      <c r="BS23" s="15"/>
-      <c r="BT23" s="15"/>
-      <c r="BU23" s="15"/>
-      <c r="BV23" s="15"/>
-      <c r="BW23" s="15"/>
-      <c r="BX23" s="15"/>
-      <c r="BY23" s="15"/>
-      <c r="BZ23" s="15"/>
-      <c r="CA23" s="15"/>
-      <c r="CB23" s="15"/>
-      <c r="CC23" s="15"/>
-      <c r="CD23" s="15"/>
-      <c r="CE23" s="15"/>
-      <c r="CF23" s="15"/>
-      <c r="CG23" s="15"/>
-      <c r="CH23" s="15"/>
-      <c r="CI23" s="15"/>
-      <c r="CJ23" s="15"/>
-      <c r="CK23" s="15"/>
-      <c r="CL23" s="15"/>
-      <c r="CM23" s="15"/>
-      <c r="CN23" s="15"/>
-      <c r="CO23" s="15"/>
-      <c r="CP23" s="15"/>
-      <c r="CQ23" s="15"/>
-      <c r="CR23" s="15"/>
-      <c r="CS23" s="15"/>
-      <c r="CT23" s="15"/>
-      <c r="CU23" s="15"/>
-      <c r="CV23" s="15"/>
-      <c r="CW23" s="15"/>
-      <c r="CX23" s="15"/>
-      <c r="CY23" s="15"/>
-      <c r="CZ23" s="15"/>
+    <row r="24" spans="1:104" s="16" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="15"/>
+      <c r="AL24" s="15"/>
+      <c r="AM24" s="15"/>
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="15"/>
+      <c r="AP24" s="15"/>
+      <c r="AQ24" s="15"/>
+      <c r="AR24" s="15"/>
+      <c r="AS24" s="15"/>
+      <c r="AT24" s="15"/>
+      <c r="AU24" s="15"/>
+      <c r="AV24" s="15"/>
+      <c r="AW24" s="15"/>
+      <c r="AX24" s="15"/>
+      <c r="AY24" s="15"/>
+      <c r="AZ24" s="15"/>
+      <c r="BA24" s="15"/>
+      <c r="BB24" s="15"/>
+      <c r="BC24" s="15"/>
+      <c r="BD24" s="15"/>
+      <c r="BE24" s="15"/>
+      <c r="BF24" s="15"/>
+      <c r="BG24" s="15"/>
+      <c r="BH24" s="15"/>
+      <c r="BI24" s="15"/>
+      <c r="BJ24" s="15"/>
+      <c r="BK24" s="15"/>
+      <c r="BL24" s="15"/>
+      <c r="BM24" s="15"/>
+      <c r="BN24" s="15"/>
+      <c r="BO24" s="15"/>
+      <c r="BP24" s="15"/>
+      <c r="BQ24" s="15"/>
+      <c r="BR24" s="15"/>
+      <c r="BS24" s="15"/>
+      <c r="BT24" s="15"/>
+      <c r="BU24" s="15"/>
+      <c r="BV24" s="15"/>
+      <c r="BW24" s="15"/>
+      <c r="BX24" s="15"/>
+      <c r="BY24" s="15"/>
+      <c r="BZ24" s="15"/>
+      <c r="CA24" s="15"/>
+      <c r="CB24" s="15"/>
+      <c r="CC24" s="15"/>
+      <c r="CD24" s="15"/>
+      <c r="CE24" s="15"/>
+      <c r="CF24" s="15"/>
+      <c r="CG24" s="15"/>
+      <c r="CH24" s="15"/>
+      <c r="CI24" s="15"/>
+      <c r="CJ24" s="15"/>
+      <c r="CK24" s="15"/>
+      <c r="CL24" s="15"/>
+      <c r="CM24" s="15"/>
+      <c r="CN24" s="15"/>
+      <c r="CO24" s="15"/>
+      <c r="CP24" s="15"/>
+      <c r="CQ24" s="15"/>
+      <c r="CR24" s="15"/>
+      <c r="CS24" s="15"/>
+      <c r="CT24" s="15"/>
+      <c r="CU24" s="15"/>
+      <c r="CV24" s="15"/>
+      <c r="CW24" s="15"/>
+      <c r="CX24" s="15"/>
+      <c r="CY24" s="15"/>
+      <c r="CZ24" s="15"/>
     </row>
-    <row r="24" spans="1:104" x14ac:dyDescent="0.2">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="30" spans="1:104" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
+    <row r="25" spans="1:104" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="31" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
@@ -5955,6 +5985,9 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B6">
@@ -5985,7 +6018,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:B20">
+  <conditionalFormatting sqref="B19:B21">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -6008,6 +6041,7 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="14" max="29" man="1"/>
   </colBreaks>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -6048,10 +6082,49 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B19:B20</xm:sqref>
+          <xm:sqref>B19:B21</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C666497-1730-44BD-81C1-BF7FA517501B}">
+  <dimension ref="B1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>